<commit_message>
Writer demo files uploaded
Writer demo files uploaded; I do not plan on having a PowerPoint for this part of the presentation, just a live demo (as described in Presentation Script.docs)
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Any dates before Feb 28, 1900 are one day off</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Read qvx files directly from the internet</t>
   </si>
   <si>
-    <t>Solution</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Regular expression fix</t>
   </si>
   <si>
-    <t>Saturday</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -87,7 +81,7 @@
     <t>Deal with missing cells (esp. with dates from strings,and verify nothing else was broken by this)</t>
   </si>
   <si>
-    <t>Establish and run test cases</t>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -449,19 +443,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="81.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.21875" customWidth="1"/>
+    <col min="1" max="1" width="85" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -469,125 +462,117 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="B14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>